<commit_message>
Remove videos from Git tracking and update config/data files
</commit_message>
<xml_diff>
--- a/public/data/New_Book.xlsx
+++ b/public/data/New_Book.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$E$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$E$144</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="330">
   <si>
     <t>Shri Ajay Jain</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Shri Vinod Fandot</t>
   </si>
   <si>
-    <t>Shri Ashish Jain(Babu Ji)</t>
-  </si>
-  <si>
     <t>Shri Pawan Sanjay Jain (Moti Sans)</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Shri Hukmi Chand ji Shanti lal ji Shah</t>
   </si>
   <si>
-    <t>Shri Hira lal ji Mukesh Kumar Kachrawat</t>
-  </si>
-  <si>
     <t>Indore</t>
   </si>
   <si>
@@ -248,24 +242,12 @@
     <t>Mob</t>
   </si>
   <si>
-    <t xml:space="preserve">Eramik Silwasa Ltd. Pipariya Industrial, Silwasa (Dadar &amp; Nagar Haveli) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A-355, Suryanagar, Ghaziabad (U.P.) 201011 , </t>
-  </si>
-  <si>
     <t xml:space="preserve">403, Royal Charch, 56 South Tuko Ganj Treasure Island Indore, (M.P.) </t>
   </si>
   <si>
     <t xml:space="preserve">Nagori Pathologi Ke Samne, Deedwana, Oli Sarafa Bazar, Lashkar Gwalior (M.P.) </t>
   </si>
   <si>
-    <t xml:space="preserve">63, Suraj Nagar, Model town, Delhi 110009, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chironji lal ka Bada, Dal bazar, Gwalior (M.P.) 474009, </t>
-  </si>
-  <si>
     <t>Shri Dr.V.K.Jain Jain</t>
   </si>
   <si>
@@ -275,54 +257,21 @@
     <t>Shri Mahindra Nigotiya</t>
   </si>
   <si>
-    <t>Shri Askash jain, Prakash jain (parash chennal)</t>
-  </si>
-  <si>
     <t>Shri Pradeep Jain (Mahaveera Chennal)</t>
   </si>
   <si>
-    <t>Shri Rakesh manju &amp; Associates (C.A.)</t>
-  </si>
-  <si>
     <t>Shri Indra Kumar Sethi</t>
   </si>
   <si>
-    <t>Shri Rakesh ji,Basanti lal ji jain</t>
-  </si>
-  <si>
     <t>Shri Ajay Ji Jain</t>
   </si>
   <si>
-    <t>Shri  Pradyuman ji</t>
-  </si>
-  <si>
-    <t>Shri  Pradeep ji</t>
-  </si>
-  <si>
-    <t>Shri Rahul ji kasliwal (advocate)</t>
-  </si>
-  <si>
-    <t>Shri vishal ji badjatiya</t>
-  </si>
-  <si>
-    <t>Shri Vilas ji kasliwal</t>
-  </si>
-  <si>
-    <t>Shri Jitender ji agarwal</t>
-  </si>
-  <si>
     <t>Mantri</t>
   </si>
   <si>
     <t>Shri Pradeep Jain 'Mama'</t>
   </si>
   <si>
-    <t>Sanghpati and Sanrakshak  Shiromani</t>
-  </si>
-  <si>
-    <t>A-1 Pratibha villa, Raj Evenue, Chuna Bhatti, Bhopal  (M.P.)</t>
-  </si>
-  <si>
     <t>Sanrakshak Shiromani</t>
   </si>
   <si>
@@ -332,9 +281,6 @@
     <t>Shri Vinod Jain 'Koyle Wale'</t>
   </si>
   <si>
-    <t>Mangal Shri Palace Krantinagar, Bilaspur,Chhatisgarh</t>
-  </si>
-  <si>
     <t>Shri Kushal Tholia</t>
   </si>
   <si>
@@ -350,9 +296,6 @@
     <t>Karyashyaksh</t>
   </si>
   <si>
-    <t>Shri Vinod Jain</t>
-  </si>
-  <si>
     <t>Upadhyaksh</t>
   </si>
   <si>
@@ -362,9 +305,6 @@
     <t>Mahamantri</t>
   </si>
   <si>
-    <t>Shri Ajit VinayakyaShri Ajit Vinayakya</t>
-  </si>
-  <si>
     <t>Koshyadhyaksh</t>
   </si>
   <si>
@@ -374,114 +314,21 @@
     <t>Designation</t>
   </si>
   <si>
-    <t>9-7 Scheme No. 71, Gumasta Nagar Behind Community Hall, Indore  (M.P.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A-161/162, Park Plaza New Yaari Road ,Varsova Andheri, Mumbai (MH.) </t>
-  </si>
-  <si>
-    <t>B-1, C-1 Somnath dev Socity, Sargam Shopping Ke Pichche Lok Bharti School Ke Samne Parle Point, Surat</t>
-  </si>
-  <si>
-    <t>A-203-204, Pulak sangam niwas, shyam vatika township, Near Modal town, Parwat Patiya, Surat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supvi Parivar Aprt. 306, Poineer Hospital, Ke Pass Station Road, Sikar (Raj) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B-1, C-1 Somnath dev Socity Sargam Shopping Ke Pichche, Lok Bharti School Ke, Samne Parle Point Surat (Guj) </t>
-  </si>
-  <si>
-    <t>B-9 C-Scheme, Vivekanand Marg, Jaipur (Raj)</t>
-  </si>
-  <si>
-    <t>29-30, Paliwal Nagar, Indore (M.P.)</t>
-  </si>
-  <si>
-    <t>202, Mansarovar Mount Pleasant Road, Malabar Hill, Mumbai, (MH.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 ,Bhaveshwar Darshan, 3Rd Floor, Altamount, Road Mumbai (MH.) </t>
-  </si>
-  <si>
-    <t>102 ,B Jadon Nagar, Veer Nagar, Jaipur (Raj)</t>
-  </si>
-  <si>
-    <t>Sitola Sahab Ka Vada ,Darji Oli, Lashkar Gwalior (M.P.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B Ground Floor,No. 2701 ,Vyumand Bldg, Saheb Marathe Marg, Prabhadevi ,Mumbai (M.H.) </t>
-  </si>
-  <si>
-    <t>A-13, Jai Jawan Colony 1 ,Tonk Road, Jaipur (Raj)</t>
-  </si>
-  <si>
-    <t>B- Wing ,Flat No. 2501, Lodha Velisimo N.M. Joshi Marg ,Apolo Mill Compound ,Mumbai (MH.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74, Jai Jawan Colony 2, Jaipur (Raj) , </t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.M. Memorial Jain Heart &amp; General Hospital, Station Road ,Sikar (Raj) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nimpal Kar Ke Gate No. 2 Vihar Aprt, Nancha Bazar, Gwalior ( M.P.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B-75 ,Kirti Nagar, Near Jain Mandir, Tonk Road, Jaipur (Raj) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Flat No. 02, Ground Floor, Frankoniya Bldg, Pasta Len Kalwa, Mumbai (MH.) </t>
   </si>
   <si>
-    <t xml:space="preserve">Manjula Sadan (Panwala) 8, Mahatma Gandhi Socity ,Opp-Dharma Row House, Near Monalisha, Aprt Surat (Guj) </t>
-  </si>
-  <si>
-    <t>527, Anmol Market ,Near Raghukul Market, Ring Road, Surat (Guj)</t>
-  </si>
-  <si>
     <t xml:space="preserve">D-216, Surya Prakash Residency, City Light, Surat (Guj) </t>
   </si>
   <si>
-    <t xml:space="preserve">536, 5th Floor,Velgyum Tower, Delhi Gate ,Ring Road Surat (Guj) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumar Silk Mills, O- 3259/60 ,S.T.M Ring Road, Surat (Guj) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jagrati Encleve, Delhi 92 , </t>
-  </si>
-  <si>
     <t>34/35, Shivam Bldg. Plot No. 4, Rdp-5, Sec-7 Baba Saheb Amvedkar Road Near Charkop Bus Depo &amp; Sarswati Hospital Kandivali (W), Mumbai (MH.)</t>
   </si>
   <si>
-    <t>D-24/25, Subhash Marg ,C-Sceam ,Jaipur (Raj)</t>
-  </si>
-  <si>
-    <t>D-10, Balram Nagar Loni, Ghaziabad (U.p.)</t>
-  </si>
-  <si>
     <t>Chandukaka Sarof &amp; Sons Pvt.Ltd, Baramati (MH.)</t>
   </si>
   <si>
-    <t>Ajink Bazar Bhivgan Road,Baramati (MH.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">305, Tulip Residency, Opp-Navasha Maruti, Near Bank Of India, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.D. Shri Emporiyam Pvt. 2, Hariram Goynka Street, </t>
-  </si>
-  <si>
-    <t>Flt No.1002/1003,B-Wing, Palm Beach,Residency Amey C.H.S. LTD. ,Plot no. 24 Sec- 4 Nerul, Navi Mumbai</t>
-  </si>
-  <si>
     <t>Hiraman Tower, Govardhan Vilas, Floor-10th, Udaipur (Raj) 313001</t>
   </si>
   <si>
-    <t>8 ,Mehta Ji Ki Vadi, Gulab Baug ,Udaipur (Raj)</t>
-  </si>
-  <si>
     <t>166, Vakil Colony, Sec-11, Udaipur (Raj)</t>
   </si>
   <si>
@@ -494,288 +341,93 @@
     <t>Golcha Marg, Sadar Nagar, Nagpur (MH.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Agriko Industrial Area ,Javara-Ratlam, (M.P.) 457726, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sapna Agency, Sapna Bldg. Near P.D. Company, </t>
-  </si>
-  <si>
-    <t>A-108 Anal Aprt, Vijay Char Rasta ,Opp-Honest Restaurant, Ahamdabad (Guj)</t>
-  </si>
-  <si>
     <t>Bahubali Colony, Near- Jain Mandir, Bansvada (Raj)</t>
   </si>
   <si>
-    <t>172-E Block ,Adarsh Nagar, Kalka Mata Road Udaipur (Raj)</t>
-  </si>
-  <si>
-    <t>Tara Bhavan, 6-7 Near Sarvritu Vilas Park, Udaipur(Raj)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2678, Bholanath Nagar, Shahdra, Delhi, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swastik 29-30, Utkarsh Vihar, Near Manish Puri Khajrana Road, </t>
-  </si>
-  <si>
     <t>43, Ramchandra Nagar Extension, Airodram Road, Indore</t>
   </si>
   <si>
-    <t xml:space="preserve">B-134, Swasth Vihar, Delhi 110092 , </t>
-  </si>
-  <si>
-    <t>Kushal bagh, Banswara, (Raj)</t>
-  </si>
-  <si>
     <t>105-106, Kothari Bhawan Near Dr.Kothari Clinic Commercial Colony, Banswara, (Raj)</t>
   </si>
   <si>
-    <t>R.K. Jewellers , Banswara (Raj)</t>
-  </si>
-  <si>
     <t>Nasik</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kopergaon</t>
-  </si>
-  <si>
-    <t>House No. 234, front off Janak Puri, Place Jiwaji Gunj, Lashkar,Gwalior</t>
-  </si>
-  <si>
     <t>Trustee</t>
   </si>
   <si>
     <t>Udaipur</t>
   </si>
   <si>
-    <t>Shri Rajesh, smt. anita Ravka</t>
-  </si>
-  <si>
     <t>Shri Ankit Jain</t>
   </si>
   <si>
     <t xml:space="preserve">M-10, Sagar Vihar Colony Vaishali Nagar Ajmer (Raj) </t>
   </si>
   <si>
-    <t xml:space="preserve">Shri Ajay, smt. Sarita Jain </t>
-  </si>
-  <si>
-    <t>B-1, C-1 Somnath dev Socity Sargam Shahdra Delhi-110009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shri Niramal swaroop, smt. nirmala Jain </t>
-  </si>
-  <si>
-    <t>Shri Sudip, smt. Rashmi Jain</t>
-  </si>
-  <si>
     <t>Ajmer Ayran Industry Area, Parvatpura Ajmer (Raj)</t>
   </si>
   <si>
     <t>Arihant Group Banswara, (Raj)</t>
   </si>
   <si>
-    <t>2504, Maru Ji Ka Chowk Motisingh Bhamiyo Ka Rasta Johri Bazar,Jaipur,  (Raj)</t>
-  </si>
-  <si>
-    <t>H-2504 MSB ka rasta maru ji ka chock Johri bazar,Jaipur- 327001,(Raj)</t>
-  </si>
-  <si>
-    <t>143, Hiran Margi Sec- 11,jain mandir ke pichhe, Udaipur (Raj)</t>
-  </si>
-  <si>
     <t>188, Tegore Nagar, Hiran Margi Senp Udaipur (Raj)</t>
   </si>
   <si>
     <t>Shri Vimal Kumar</t>
   </si>
   <si>
-    <t>Shopping Ke Pichche Lok Bharti School Ke,Gwalior-474001,(M.P.)</t>
-  </si>
-  <si>
-    <t>Matawali Gali, Krishnapura ,Murar Gwalior-474006 (M.P.)</t>
-  </si>
-  <si>
     <t>Radakrisan Market, Sarafa Bazar, Grater (Lashkar) Gwalior, (M.P.)</t>
   </si>
   <si>
     <t>Shri Yogita Ritesh Ajmera</t>
   </si>
   <si>
-    <t>Swastik 29-30 Utkarsh Vihar Nr- Manish Puri Khajrana Road Indore (M.P)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shruti Shoot llp, 275 M.T. Clock Market, Indore, </t>
-  </si>
-  <si>
     <t>152, Gumasta Nagar, Indore- 452009, (M.P.)</t>
   </si>
   <si>
-    <t>35/1 sneh lata ganj near kyorvel school Indore</t>
-  </si>
-  <si>
-    <t>Shri Sunil smt. rakhi Kothari</t>
-  </si>
-  <si>
-    <t>Shri Deepak, smt. Vandna jain</t>
-  </si>
-  <si>
     <t>Bhaichand Jyoti Chand Saraf, Baramati, Pune (MH.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Flat No. 102, A Wing, City Pride Sahakar Chowk, Kurkumbh Road, Daund, Pune   (MH.) 413801, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niranjan Park, Manik Bagh, Singhgad Road, Pune   (MH.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rmd House 64, Koregaon Park ,Lane No.3, Pune   411001 (MH.) </t>
-  </si>
-  <si>
-    <t>Hridyam,291- A, Hiran Mangri, Sec no. 11, Udaipur (Raj)</t>
-  </si>
-  <si>
-    <t>2 C- 201, Nehru Nagar, Ghaziabad (U.P.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B- 134 A (M.H.),veer Marg Ambawadi, Marg Jaipur (Raj) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-C / 46, New Rohtak Road ,Karol Bagh, New Delhi 05, </t>
-  </si>
-  <si>
     <t>1087, Gyan Nagar Hiran Magri, Sec-4, Udaipur (Raj)</t>
   </si>
   <si>
     <t xml:space="preserve">Arpna Banglow, Plot No.24, Sahyog Soceity, Bhigvan Road, Baramati, Pune- 413102 (MH.) </t>
   </si>
   <si>
-    <t>Vishal Height C/O Brahma Pure Veg, S.No. 39/2 Manik Bagh, Sinhggad Road,Pune  - 411051 (MH.)</t>
-  </si>
-  <si>
     <t>Pushp Pulak Nilay, A- 34, Kirti Nagar, Tonk Road, Jaipur (Raj)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bharat Electronics, Udaipur Road, Shiv colony, Opp- Income, </t>
-  </si>
-  <si>
-    <t>Nr- Bright Star School V.O.C. Gate, bahu bazar  North- Vogaigaon Assam 783380</t>
-  </si>
-  <si>
-    <t>Rishav Pariwar- G-131 preet vihar behind jhankar benqet hall delhi</t>
-  </si>
-  <si>
     <t>G- 169, Prajapat Nagar, Goutam Nagar, New Delhi</t>
   </si>
   <si>
-    <t>Shri Sunil . Smt. Saroj kala</t>
-  </si>
-  <si>
-    <t>plot no 17 Ahinsa nagar aakshvani ke saamne, Aurngabad (MH.)</t>
-  </si>
-  <si>
-    <t>Shri sunil, sou. mona pandey</t>
-  </si>
-  <si>
-    <t>Rachna traiders, jain mandir ke samne, Raja bazar,Aurngabad (MH.)</t>
-  </si>
-  <si>
-    <t>Shri Nilesh (pintu) sou. Shalaka patni</t>
-  </si>
-  <si>
-    <t>G9,Kasliwal vihar,Pratapnagar, Osmanpura,Auranagabad-431001,(MH.)</t>
-  </si>
-  <si>
-    <t>Shri Sushil, Sou. sushmita Shah</t>
-  </si>
-  <si>
-    <t>Rajabazar kuwarfully shanti niley,Aurngabad (MH.)</t>
-  </si>
-  <si>
     <t>Flat No. 102, A Wing, City Pride Sahakar Chowk, Kurkumbh Road Daund, Pune-413801, (MH.)</t>
   </si>
   <si>
-    <t>Shri Pankaj Ji, smt. Padma Jain (itra wale)</t>
-  </si>
-  <si>
     <t>43, Vaatsaly, 6-N-S Road, J.P.D Scheme Vileparle Mumbai (M.H.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Prakash Tower ,66 Swastik Socity,5th Road, J.B.P.D Mumbai (MH.)-400056, </t>
-  </si>
-  <si>
-    <t>Unit No. 412A, 4th Floor, The Capital, C-70, G-Block, Bandra Kurla Complex, Bandra (E) Mumbai - 400051,(MH.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andheri Lokhanwala 71, Neminath lixeria , 1103/04 SVP nagar mhada telephone exchange near food villas restrorant andheri west Mumbai-400053 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Shri Hemant Bohra </t>
   </si>
   <si>
-    <t>Sonam Aprt, Flt No.103/104, Kartar Road No.3, Borivali East- 400066(MH.)</t>
-  </si>
-  <si>
-    <t>Kurla Andheri Road MIDC Mumbai(MH.)</t>
-  </si>
-  <si>
-    <t>Aachal bunglow,Plot no.58, secno.1, charkop, Kandivali West Mumbai-400067 (M.H.)</t>
-  </si>
-  <si>
-    <t>Shri Rajesh, smt. Vimla devi Shah</t>
-  </si>
-  <si>
     <t>Niranjan Park, Manik Baug, Singhgad Road Manik Baug - Pune (MH.)</t>
   </si>
   <si>
-    <t>79, Ratntry Bhavani Peth, Gul Ali, Pune -411002,    (MH.)</t>
-  </si>
-  <si>
-    <t>Shri Naveen, sou. Ujjwala patni</t>
-  </si>
-  <si>
     <t>Aurngabad (MH.)</t>
   </si>
   <si>
-    <t>Dr. Vinay jain</t>
-  </si>
-  <si>
-    <t>9th floor, Kalpataru Regalia, Opp. Inorbit Mall, off Link Road, Malad West, Mumbai 64 (MH.)</t>
-  </si>
-  <si>
     <t>Shri Suresh Kusum Chhabra</t>
   </si>
   <si>
     <t>Mumbai (MH.)</t>
   </si>
   <si>
-    <t>Shri Manoj priyanka badjatya</t>
-  </si>
-  <si>
-    <t>Shri Vikas Reema sethi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301 the prakview opp, mahila muncipal gardan, rajpath B/H, rajpath rangoli road bodadev Ahemdabaad-380054 Gujrat </t>
-  </si>
-  <si>
-    <t>Bangla no-06 Opera House City Light Surat(Guj)</t>
-  </si>
-  <si>
     <t>Shri Praveen, Smt. Beena Jain</t>
   </si>
   <si>
     <t>Shri Nirmal Badjatya</t>
   </si>
   <si>
-    <t>Shri Ajit, smt. shashi jain</t>
-  </si>
-  <si>
-    <t>8- HILL VIEW PARK BY. PAAS ROAD SARIGAM - UMAR GAON DISS. VALSAD(Guj)</t>
-  </si>
-  <si>
-    <t>Shri Mayank ji Mahaveer Ji Pichori</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shri Pushpender Ji Vinita Ji Hinsawat </t>
   </si>
   <si>
@@ -809,54 +461,12 @@
     <t>Borawke nagar Ward no 7 Shrirampur Dist Ahmadnagar(MH.)</t>
   </si>
   <si>
-    <t>Kalpana Housing Society , Behind kala Ram mandir Ward no- 7 (Shrirampur)(MH.)</t>
-  </si>
-  <si>
-    <t>Shri Pradeep, smt. Kamlesh sethi</t>
-  </si>
-  <si>
-    <t>Shri Alok, smt. Archana jain</t>
-  </si>
-  <si>
-    <t>Shri Pramod, sou. Urmila tholey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shri Prasad, sou. Deepti patni </t>
-  </si>
-  <si>
     <t>Shri Suman Ashok Gangwal</t>
   </si>
   <si>
     <t>Shri Apurva Naresh Kumar Soni</t>
   </si>
   <si>
-    <t>Shri Ashok, Jyoti jain</t>
-  </si>
-  <si>
-    <t>Shri Sohan lal, smt. asha vidavat</t>
-  </si>
-  <si>
-    <t>Shri Ashish ji, smt. Sarita jain suthwala</t>
-  </si>
-  <si>
-    <t>Shri Pratipal ji, smt. kusum tongiya</t>
-  </si>
-  <si>
-    <t>Shri Suresh, Smt. meena mehta</t>
-  </si>
-  <si>
-    <t>Shri  Vishal khushboo ji tholiya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shri Mangilal ji kothari </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shri Ashok ji bohra </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shri Suresh ji sanghvhi </t>
-  </si>
-  <si>
     <t>Smt. Shobha Tai Rasiklal Ji Dhariwaal</t>
   </si>
   <si>
@@ -878,75 +488,501 @@
     <t>Shri Anil Neera Jain</t>
   </si>
   <si>
-    <t>175/176 saurabh society GIDC VAPI DIST VALSAD (Guj)</t>
-  </si>
-  <si>
-    <t>Nirala bazar maharashtra (MH.)</t>
-  </si>
-  <si>
-    <t>Flt No.1002/1003,B-Wing, Palm Beach,Residency Amey C.H.S. LTD. Plot no. 24 Sec- 4 Nerul, Navi Mumbai (MH.)</t>
-  </si>
-  <si>
-    <t>73/gumasta nagar, main road  452009 Indore</t>
-  </si>
-  <si>
-    <t>Hridyam 291,Hiran Magri,Sec no.11,Udaipur(Raj)</t>
-  </si>
-  <si>
-    <t>55, Sarav Ritu Vilas,Udaipur (Raj)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 98377 47950</t>
-  </si>
-  <si>
-    <t>Main Parshav Pustak Mandir,Neta Subhash Margh,Bans Mandi,Etah</t>
-  </si>
-  <si>
-    <t>46-B,Sarvritu Vilas,Park ke samne,Udaipur(Raj)</t>
-  </si>
-  <si>
-    <t>Mahaveer Nagar,Baapu Bazar,'Kavita Kutir',Rishabhdev,Udaipur(Raj)</t>
-  </si>
-  <si>
-    <t>1403/4, Edenwoods,Shastri Nagar,Near Lokhandwala Circle,Andheri west,Mumbai (MH.)</t>
-  </si>
-  <si>
-    <t>581, Khatiwala Tank,near Tower,Choraha,Indore(M.P.)</t>
-  </si>
-  <si>
-    <t>Shri Digamber Jain Jinsharnam Teerthdham trust(Reg.),Agricho Industrial Area,Javara-457726(M.P.)</t>
-  </si>
-  <si>
-    <t>Shri Digamber Jain Jinsharnam Teerthdham trust(Reg.), Rmd House 64,Koregaon Park,Lane No.3,Pune (MH.)411001</t>
-  </si>
-  <si>
-    <t>Hno.3, MUNICIPAL COLONY, SHIVAJI NADAR Udaipur</t>
-  </si>
-  <si>
     <t>Jaipur</t>
   </si>
   <si>
-    <t xml:space="preserve">Beej bhandar 110 nandlal pura sabji mandi Indore </t>
-  </si>
-  <si>
-    <t>9,Mohini vila,Anmol Alience Colony Near Celebration Mall Udaipur (Raj) 313001</t>
-  </si>
-  <si>
-    <t>P-2, Sec. 14, 100ft. Road, Near Mahaveer Tower Udaipur</t>
-  </si>
-  <si>
-    <t>Colony Vaedaan Mahaveer School Pagalyaji Road, Rishabhdev,Udaipur(Raj)</t>
-  </si>
-  <si>
-    <t>Madhuvan Villa, H.No.3 , Municipal Colony ,Shivaji Nagar,Udaipur,  Rajasthan</t>
-  </si>
-  <si>
-    <t>16, aashish nager hiran managri sec.5 sai baba road udaipur rajasthan 313002</t>
+    <t>Shri Ajit Vinayakya</t>
+  </si>
+  <si>
+    <t>RMD House No. 64, Lane No. 3, Koregaon Park, Pune – 411001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2504, Maru Ji Ka Chowk, Motisingh Bhamiyo Ka Rasta, Johri Bazar, Jaipur – 302003, (Raj) </t>
+  </si>
+  <si>
+    <t>9/7, Scheme No. 71, Gumasta Nagar, Behind Community Hall, Indore, (M.P.)</t>
+  </si>
+  <si>
+    <t>B-1, C-1, Somnath Dev Society, Sargam Shopping Ke Pichhe, Lok Bharti School Ke Samne, Parle Point, Surat</t>
+  </si>
+  <si>
+    <t>Hridyam, 291, Hiran Magri, Sector No. 11, Udaipur, (Raj)</t>
+  </si>
+  <si>
+    <t>Swastik, 29–30, Utkarsh Vihar, Near Manish Puri, Khajrana Road, Indore – 452016, (M.P.)</t>
+  </si>
+  <si>
+    <t>A-203–204, Pulak Sangam Niwas, Shyam Vatika Township, Near Model Town, Parvat Patiya, Surat (Guj)</t>
+  </si>
+  <si>
+    <t>Supvi Parivar Apartment, 306, Near Pioneer Hospital, Station Road, Sikar, (Raj)</t>
+  </si>
+  <si>
+    <t>Eramik Silvassa Ltd., Pipariya Industrial Area, Silvassa, Dadra and Nagar Haveli and Daman and Diu</t>
+  </si>
+  <si>
+    <t>B-9, C-Scheme, Vivekanand Marg, Jaipur – 302001, (Raj)</t>
+  </si>
+  <si>
+    <t>29–30, Paliwal Nagar, Indore – 452001, (M.P.)</t>
+  </si>
+  <si>
+    <t>202, Mansarovar, Mount Pleasant Road, Malabar Hill, Mumbai – 400006, (MH.)</t>
+  </si>
+  <si>
+    <t>16, Bhaveshwar Darshan, 3rd Floor, Altamount Road, Mumbai – 400026, (MH.)</t>
+  </si>
+  <si>
+    <t>17, A-2, Great Eastern Royal, 333 Bellasis Bridge, Tardeo, Mumbai – 400034, (MH.)</t>
+  </si>
+  <si>
+    <t>2, C-201, Nehru Nagar, Ghaziabad – 201001, (UP.)</t>
+  </si>
+  <si>
+    <t>102, B Jadon Nagar, Veer Nagar, Jaipur – 302004, (Raj)</t>
+  </si>
+  <si>
+    <t>B Ground Floor, No. 2701, Vyumand Building, Saheb Marathe Marg, Prabhadevi, Mumbai – 400025, (MH.)</t>
+  </si>
+  <si>
+    <t>A-13, Jai Jawan Colony 1, Tonk Road, Jaipur – 302015, (Raj)</t>
+  </si>
+  <si>
+    <t>B-Wing, Flat No. 2501, Lodha Velisimo, N.M. Joshi Marg, Apollo Mill Compound, Mumbai – 400011, (MH.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4, Jai Jawan Colony 2, Jaipur – 302015, (Raj) </t>
+  </si>
+  <si>
+    <t>K.M. Memorial Jain Heart &amp; General Hospital, Station Road, Sikar – 332001, (Raj)</t>
+  </si>
+  <si>
+    <t>Nimpal Kar, Gate No. 2, Vihar Apartment, Nancha Bazar, Gwalior – 474001, (M.P.)</t>
+  </si>
+  <si>
+    <t>B-134 A, Veer Marg, Ambawadi, Jaipur – 302006, (Raj)</t>
+  </si>
+  <si>
+    <t>Shri Rakesh Manju &amp; Associates (C.A.)</t>
+  </si>
+  <si>
+    <t>Shri Askash Jain, Prakash jain (Parash Chennal)</t>
+  </si>
+  <si>
+    <t>Shri Hira lal Ji Mukesh Kumar Kachrawat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Suresh Ji Sanghvhi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Ashok Ji Bohra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Mangilal Ji Kothari </t>
+  </si>
+  <si>
+    <t>Shri Rahul Ji Kasliwal (Advocate)</t>
+  </si>
+  <si>
+    <t>Shri Vishal Ji Badjatiya</t>
+  </si>
+  <si>
+    <t>Shri Vilas Ji Kasliwal</t>
+  </si>
+  <si>
+    <t>Shri Jitender Ji Agarwal</t>
+  </si>
+  <si>
+    <t>Shri Rajesh, Smt. Anita Ravka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Ajay, Smt. Sarita Jain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Niramal Swaroop, Smt. Nirmala Jain </t>
+  </si>
+  <si>
+    <t>Shri Sudip, Smt. Rashmi Jain</t>
+  </si>
+  <si>
+    <t>Shri Mayank Ji Mahaveer Ji Pichori</t>
+  </si>
+  <si>
+    <t>Shri Suresh, Smt. Meena Mehta</t>
+  </si>
+  <si>
+    <t>Shri Pratipal Ji, Smt. Kusum Tongiya</t>
+  </si>
+  <si>
+    <t>Shri Pradeep, Smt. Kamlesh Sethi</t>
+  </si>
+  <si>
+    <t>Shri Ashish Ji, Smt. Sarita Jain Suthwala</t>
+  </si>
+  <si>
+    <t>Shri Sunil Smt. Rakhi Kothari</t>
+  </si>
+  <si>
+    <t>Shri Deepak, Smt. Vandna Jain</t>
+  </si>
+  <si>
+    <t>Shri Pankaj Ji, Smt. Padma Jain (Itra Wale)</t>
+  </si>
+  <si>
+    <t>Shri Sohan Lal, Smt. Asha Vidavat</t>
+  </si>
+  <si>
+    <t>Shri Alok, Smt. Archana Jain</t>
+  </si>
+  <si>
+    <t>Shri Rajesh, Smt. Vimla Devi Shah</t>
+  </si>
+  <si>
+    <t>Dr. Vinay Jain</t>
+  </si>
+  <si>
+    <t>Shri Manoj Priyanka Badjatya</t>
+  </si>
+  <si>
+    <t>Shri Vikas Reema Sethi</t>
+  </si>
+  <si>
+    <t>Shri Ashok, Jyoti Jain</t>
+  </si>
+  <si>
+    <t>Shri Ajit, Smt. Shashi Jain</t>
+  </si>
+  <si>
+    <t>Shri Sunil, Smt. Saroj Kala</t>
+  </si>
+  <si>
+    <t>Shri Sunil, Smt. Mona Pandey</t>
+  </si>
+  <si>
+    <t>Shri Pramod, Smt. Urmila Tholey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri Prasad, Smt. Deepti Patni </t>
+  </si>
+  <si>
+    <t>Shri Nilesh (Pintu), Smt. Shalaka Patni</t>
+  </si>
+  <si>
+    <t>Shri Sushil, Smt. Sushmita Shah</t>
+  </si>
+  <si>
+    <t>Shri Naveen, Smt. Ujjwala Patni</t>
+  </si>
+  <si>
+    <t>Shri Rakesh Ji, Basanti Lal Ji Jain</t>
+  </si>
+  <si>
+    <t>Shri Vishal Khushboo Ji Tholiya</t>
+  </si>
+  <si>
+    <t>Shri Pradyuman Ji</t>
+  </si>
+  <si>
+    <t>Shri Pradeep Ji</t>
+  </si>
+  <si>
+    <t>Sanghpati and Sanrakshak Shiromani</t>
+  </si>
+  <si>
+    <t>Ajink Bazar Bhivgan Road, Baramati (MH.)</t>
+  </si>
+  <si>
+    <t>Main Parshav Pustak Mandir, Neta Subhash Margh, Bans Mandi, Etah</t>
+  </si>
+  <si>
+    <t>9, Mohini vila, Anmol Alience Colony Near Celebration Mall Udaipur (Raj) 313001</t>
+  </si>
+  <si>
+    <t>Shopping Ke Pichche Lok Bharti School Ke, Gwalior-474001, (M.P.)</t>
+  </si>
+  <si>
+    <t>Mangal Shri Palace Krantinagar, Bilaspur, Chhatisgarh (M.P.)</t>
+  </si>
+  <si>
+    <t>Sitola Sahab Ka Vada, Darji Oli, Lashkar, Gwalior – 474001, (MP)</t>
+  </si>
+  <si>
+    <t>B-75, Kirti Nagar, Near Jain Mandir, Tonk Road, Jaipur – 302015, (Raj)</t>
+  </si>
+  <si>
+    <t>Unit No. 412A, 4th Floor, The Capital, C-70, G-Block, Bandra Kurla Complex, Bandra (E) Mumbai - 400051, (MH.)</t>
+  </si>
+  <si>
+    <t>55, Sarav Ritu Vilas, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>A-1 Pratibha Villa, Raj Evenue, Chuna Bhatti, Bhopal (M.P.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niranjan Park, Manik Bagh, Singhgad Road, Pune  (MH.) </t>
+  </si>
+  <si>
+    <t>Vishal Height C/O Brahma Pure Veg, S.No. 39/2 Manik Bagh, Sinhggad Road, Pune - 411051 (MH.)</t>
+  </si>
+  <si>
+    <t>79, Ratntry Bhavani Peth, Gul Ali, Pune -411002,  (MH.)</t>
+  </si>
+  <si>
+    <t>Matawali Gali, Krishnapura, Murar Gwalior-474006 (M.P.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manjula Sadan (Panwala) 8, Mahatma Gandhi Socity, Opp-Dharma Row House, Near Monalisha, Aprt Surat (Guj) </t>
+  </si>
+  <si>
+    <t>527, Anmol Market, Near Raghukul Market, Ring Road, Surat (Guj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">536, 5th Floor, Velgyum Tower, Delhi Gate, Ring Road Surat (Guj) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumar Silk Mills, O- 3259/60, S.T.M Ring Road, Surat (Guj) </t>
+  </si>
+  <si>
+    <t>D-24/25, Subhash Marg, C-Sceam, Jaipur (Raj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rmd House 64, Koregaon Park, Lane No.3, Pune  411001 (MH.) </t>
+  </si>
+  <si>
+    <t>Flt No.1002/1003, B-Wing, Palm Beach, Residency Amey C.H.S. LTD., Plot no. 24 Sec- 4 Nerul, Navi Mumbai</t>
+  </si>
+  <si>
+    <t>8, Mehta Ji Ki Vadi, Gulab Baug, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>A-108 Anal Aprt, Vijay Char Rasta, Opp-Honest Restaurant, Ahamdabad (Guj)</t>
+  </si>
+  <si>
+    <t>172-E Block, Adarsh Nagar, Kalka Mata Road Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>R.K. Jewellers, Banswara (Raj)</t>
+  </si>
+  <si>
+    <t>Madhuvan Villa, H.No.3, Municipal Colony, Shivaji Nagar, Udaipur, Rajasthan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-161/162, Park Plaza, New Yaari Road, Varsova Andheri, Mumbai (MH.) </t>
+  </si>
+  <si>
+    <t>Vatsalya Bhavan, 4/2771, Gali No. 3, Bihari Colony, Shahdara, Delhi – 110032</t>
+  </si>
+  <si>
+    <t>A-355, Suryanagar, Ghaziabad – 201011, Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Prakash Tower, 66 Swastik Socity, 5th Road, J.B.P.D Mumbai (MH.)-400056</t>
+  </si>
+  <si>
+    <t>Jagrati Encleve, Delhi 92</t>
+  </si>
+  <si>
+    <t>3-C / 46, New Rohtak Road, Karol Bagh, New Delhi 05</t>
+  </si>
+  <si>
+    <t>D-10, Balram Nagar Loni, Ghaziabad (U.P.)</t>
+  </si>
+  <si>
+    <t>Flat No. 102, A Wing, City Pride Sahakar Chowk, Kurkumbh Road, Daund, Pune  (MH.) 413801</t>
+  </si>
+  <si>
+    <t>305, Tulip Residency, Opp-Navasha Maruti, Near Bank Of India</t>
+  </si>
+  <si>
+    <t>K.D. Shri Emporiyam Pvt. 2, Hariram Goynka Street</t>
+  </si>
+  <si>
+    <t>Agriko Industrial Area, Javara-Ratlam, (M.P.) 457726</t>
+  </si>
+  <si>
+    <t>Sapna Agency, Sapna Bldg. Near P.D. Company</t>
+  </si>
+  <si>
+    <t>2678, Bholanath Nagar, Shahdra, Delhi</t>
+  </si>
+  <si>
+    <t>Swastik 29-30, Utkarsh Vihar, Near Manish Puri Khajrana Road</t>
+  </si>
+  <si>
+    <t>B-134, Swasth Vihar, Delhi 110092</t>
+  </si>
+  <si>
+    <t>Chironji lal ka Bada, Dal bazar, Gwalior (M.P.) 474009</t>
+  </si>
+  <si>
+    <t>Shruti Shoot llp, 275 M.T. Clock Market, Indore</t>
+  </si>
+  <si>
+    <t>Bharat Electronics, Udaipur Road, Shiv colony, Opp- Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andheri Lokhanwala 71, Neminath Lixeria, 1103/04 SVP Nagar Mhada Telephone Exchange Near Food Villas Restrorant Andheri West Mumbai-400053 </t>
+  </si>
+  <si>
+    <t>Sonam Aprt, Flt No.103/104, Kartar Road No.3, Borivali East- 400066 (MH.)</t>
+  </si>
+  <si>
+    <t>Kushal Bagh, Banswara, (Raj)</t>
+  </si>
+  <si>
+    <t>Kopergaon</t>
+  </si>
+  <si>
+    <t>1403/4, Edenwoods, Shastri Nagar, Near Lokhandwala Circle, Andheri West, Mumbai (MH.)</t>
+  </si>
+  <si>
+    <t>143, Hiran Margi Sec- 11, Jain Mandir Ke Pichhe, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>House No. 234, Front Off Janak Puri, Place Jiwaji Gunj, Lashkar, Gwalior</t>
+  </si>
+  <si>
+    <t>63, Suraj Nagar, Model Town, Delhi 110009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301 The Prak View Opp, Mahila Muncipal Gardan, Rajpath B/H, Rajpath Rangoli Road Bodadev Ahmedabaad-380054 Gujrat </t>
+  </si>
+  <si>
+    <t>H-2504 MSB Ka Rasta Maru Ji Ka Chock Johri Bazar, Jaipur- 327001, (Raj)</t>
+  </si>
+  <si>
+    <t>Kalpana Housing Society, Behind Kala Ram Mandir Ward no- 7 (Shrirampur) (MH.)</t>
+  </si>
+  <si>
+    <t>Near Bright Star School V.O.C. Gate, Bahu Bazar North- Vogaigaon Assam 783380</t>
+  </si>
+  <si>
+    <t>B-1, C-1 Somnath Dev Socity Sargam, Shahdra Delhi-110009</t>
+  </si>
+  <si>
+    <t>Rishav Pariwar- G-131 Preet Vihar Behind Jhankar Banquet Hall Delhi</t>
+  </si>
+  <si>
+    <t>16, Aashish Nagar Hiran Managri Sec.5 Sai Baba Road Udaipur Rajasthan 313002</t>
+  </si>
+  <si>
+    <t>P-2, Sec. 14, 100 Ft. Road, Near Mahaveer Tower, Udaipur</t>
+  </si>
+  <si>
+    <t>H No.3, Municipal Colony, Shivaji Nagar, Udaipur</t>
+  </si>
+  <si>
+    <t>Tara Bhavan, 6-7 Near Sarvritu Vilas Park, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>46-B, Sarvritu Vilas, Park Ke Samne, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>Colony Vaedaan Mahaveer School Pagalyaji Road, Rishabhdev, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t>Mahaveer Nagar, Baapu Bazar, 'Kavita Kutir', Rishabhdev, Udaipur (Raj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beej Bhandar 110 Nandlal Pura Sabji Mandi Indore </t>
+  </si>
+  <si>
+    <t>73/Gumasta Nagar, Main Road 452009 Indore</t>
+  </si>
+  <si>
+    <t>35/1 Sneh Lata Ganj Near Kyorvel School Indore</t>
+  </si>
+  <si>
+    <t>581, Khatiwala Tank, Near Tower, Choraha, Indore(M.P.)</t>
+  </si>
+  <si>
+    <t>Shri Digamber Jain Jinsharnam Teerthdham Trust(Reg.), Agricho Industrial Area, Javara-457726 (M.P.)</t>
+  </si>
+  <si>
+    <t>Plot No 17 Ahinsa Nagar Aakshvani Ke Saamne, Aurngabad (MH.)</t>
+  </si>
+  <si>
+    <t>Nirala Bazar Maharashtra (MH.)</t>
+  </si>
+  <si>
+    <t>Rachna Traiders, Jain Mandir Ke Samne, Raja Bazar, Aurngabad (MH.)</t>
+  </si>
+  <si>
+    <t>G9, Kasliwal Vihar, Pratapnagar, Osmanpura, Auranagabad-431001, (MH.)</t>
+  </si>
+  <si>
+    <t>Rajabazar Kuwarfully Shanti Niley, Aurngabad (MH.)</t>
+  </si>
+  <si>
+    <t>Flt No.1002/1003, B-Wing, Palm Beach, Residency Amey C.H.S. Ltd. Plot No. 24 Sec- 4 Nerul, Navi Mumbai (MH.)</t>
+  </si>
+  <si>
+    <t>9th Floor, Kalpataru Regalia, Opp. Inorbit Mall, Off Link Road, Malad West, Mumbai 64 (MH.)</t>
+  </si>
+  <si>
+    <t>Kurla Andheri Road, MIDC Mumbai (MH.)</t>
+  </si>
+  <si>
+    <t>Aachal Bunglow, Plot No.58, Sec No.1, Charkop, Kandivali West, Mumbai-400067 (M.H.)</t>
+  </si>
+  <si>
+    <t>Bangla No-06 Opera House City Light, Surat (Guj)</t>
+  </si>
+  <si>
+    <t>175/176 Saurabh Society GIDC, Vapi Dist Valsad (Guj)</t>
+  </si>
+  <si>
+    <t>8- Hill View Park By Paas Road, Sarigam - Umar Gaon Dist Valsad (Guj)</t>
   </si>
   <si>
     <t>9827023894, 9425066716, 9827021894</t>
   </si>
   <si>
+    <t>98377 47950</t>
+  </si>
+  <si>
+    <t>9254900853, 8770133122</t>
+  </si>
+  <si>
+    <t>9820548120, 9821023557</t>
+  </si>
+  <si>
+    <t>9879221000, 9825800046</t>
+  </si>
+  <si>
+    <t>9893027059, 9826033179</t>
+  </si>
+  <si>
+    <t>9810900699, 6391915673</t>
+  </si>
+  <si>
+    <t>9371221365, 9423003981</t>
+  </si>
+  <si>
+    <t>9822069299, 9623025072</t>
+  </si>
+  <si>
+    <t>9325810501, 9423466988</t>
+  </si>
+  <si>
+    <t>8876520738, 9954010010</t>
+  </si>
+  <si>
+    <t>7568887806, 8094887806</t>
+  </si>
+  <si>
+    <t>9460253186, 8005591556</t>
+  </si>
+  <si>
+    <t>9414417272, 9982721430</t>
+  </si>
+  <si>
+    <t>9421242455, 9823129016</t>
+  </si>
+  <si>
+    <t>9422293966, 9823518999</t>
+  </si>
+  <si>
     <t>9425331001, 9993095558</t>
   </si>
   <si>
@@ -956,9 +992,6 @@
     <t>8003090828, 9571143143</t>
   </si>
   <si>
-    <t>9111781043 , 9425109143</t>
-  </si>
-  <si>
     <t>9869443651, 9619019591</t>
   </si>
   <si>
@@ -968,64 +1001,22 @@
     <t>9922551027, 9922434561</t>
   </si>
   <si>
-    <t>9254900853, 8770133122</t>
-  </si>
-  <si>
-    <t>9820548120, 9821023557</t>
-  </si>
-  <si>
-    <t>9879221000, 9825800046</t>
-  </si>
-  <si>
-    <t>9893027059, 9826033179</t>
-  </si>
-  <si>
-    <t>9371221365, 9423003981</t>
-  </si>
-  <si>
-    <t>9822069299, 9623025072</t>
-  </si>
-  <si>
-    <t>9325810501, 9423466988</t>
-  </si>
-  <si>
-    <t>8876520738, 9954010010</t>
-  </si>
-  <si>
-    <t>7568887806, 8094887806</t>
-  </si>
-  <si>
-    <t>9460253186, 8005591556</t>
-  </si>
-  <si>
-    <t>9414417272, 9982721430</t>
-  </si>
-  <si>
-    <t>9421242455, 9823129016</t>
-  </si>
-  <si>
-    <t>9422293966, 9823518999</t>
-  </si>
-  <si>
-    <t>9869464161 , 9987475151</t>
-  </si>
-  <si>
-    <t>8511188019 , 8976816990</t>
-  </si>
-  <si>
-    <t>9824151923 , 7878451923</t>
-  </si>
-  <si>
-    <t>9825131789 , 9825122076</t>
-  </si>
-  <si>
-    <t>812005402 , 9425347201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 A-2, great eastern royal, 333 bellasis bridge, Tardeo, Mumbai 400034(MH.) </t>
-  </si>
-  <si>
-    <t>Vatsalya Bhavan, 4/2771, Gali No 3, Bihari Colony, Shahdra, Delhi 110032</t>
+    <t>812005402, 9425347201</t>
+  </si>
+  <si>
+    <t>9824151923, 7878451923</t>
+  </si>
+  <si>
+    <t>9825131789, 9825122076</t>
+  </si>
+  <si>
+    <t>8511188019, 8976816990</t>
+  </si>
+  <si>
+    <t>9869464161, 9987475151</t>
+  </si>
+  <si>
+    <t>9111781043, 9425109143</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1193,6 +1184,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1200,8 +1194,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1484,18 +1478,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="42.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="130" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="136.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -1503,19 +1498,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,13 +1518,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>96</v>
+        <v>80</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>219</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>97</v>
+        <v>229</v>
       </c>
       <c r="E2" s="15">
         <v>9826395777</v>
@@ -1540,13 +1535,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>276</v>
+        <v>146</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>296</v>
+        <v>155</v>
       </c>
       <c r="E3" s="15">
         <v>9822242791</v>
@@ -1557,16 +1552,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>101</v>
+        <v>83</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>224</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,13 +1569,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>182</v>
+        <v>84</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="E5" s="15">
         <v>95717004183</v>
@@ -1591,16 +1586,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1608,16 +1603,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>116</v>
+        <v>246</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,16 +1620,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>117</v>
+        <v>88</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1642,13 +1637,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>287</v>
+        <v>159</v>
       </c>
       <c r="E9" s="15">
         <v>9829116369</v>
@@ -1659,16 +1654,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>191</v>
+        <v>91</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1676,33 +1671,33 @@
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="E11" s="15">
-        <v>9810900699</v>
+        <v>247</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>111</v>
+      <c r="B12" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>118</v>
+        <v>92</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>161</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1710,13 +1705,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>280</v>
+        <v>150</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="E13" s="17">
         <v>9587220111</v>
@@ -1730,10 +1725,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="E14" s="17">
         <v>7046341111</v>
@@ -1744,16 +1739,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="E15" s="17">
-        <v>9829116369</v>
+        <v>8890212345</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1761,16 +1756,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="17">
-        <v>9879221000</v>
+        <v>165</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1781,13 +1776,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="E17" s="17">
-        <v>8890212345</v>
+        <v>9867756888</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,2257 +1790,2223 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="E18" s="17">
+        <v>9460490960</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
-        <v>18</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>123</v>
+        <v>108</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>168</v>
       </c>
       <c r="E19" s="17">
-        <v>9867756888</v>
+        <v>9820134140</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="E20" s="17">
-        <v>9460490960</v>
+        <v>9810180510</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>331</v>
+        <v>108</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="E21" s="17">
-        <v>9820134140</v>
+        <v>9414056886</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="E22" s="17">
-        <v>9810180510</v>
+        <v>9425308720</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="E23" s="17">
-        <v>9414056886</v>
+        <v>9821228174</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="E24" s="17">
-        <v>9425308720</v>
+        <v>9414051102</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="E25" s="17">
-        <v>9821228174</v>
+        <v>9321135335</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>128</v>
+        <v>233</v>
       </c>
       <c r="E26" s="17">
-        <v>9414051102</v>
+        <v>9826495777</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="E27" s="17">
-        <v>9321135335</v>
+        <v>9929050403</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E28" s="17">
-        <v>9826495777</v>
+        <v>9610441111</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>130</v>
+        <v>248</v>
       </c>
       <c r="E29" s="17">
-        <v>9929050403</v>
+        <v>7838166822</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="E30" s="17">
-        <v>9610441111</v>
+        <v>9301100201</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="E31" s="17">
-        <v>7838166822</v>
+        <v>9829019301</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>132</v>
+        <v>226</v>
       </c>
       <c r="E32" s="17">
-        <v>9301100201</v>
+        <v>9413180225</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>203</v>
+        <v>95</v>
       </c>
       <c r="E33" s="17">
-        <v>9829019301</v>
+        <v>9820402573</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="17">
-        <v>9413180225</v>
+        <v>234</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E35" s="17">
-        <v>9820402573</v>
+        <v>235</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>328</v>
+        <v>96</v>
+      </c>
+      <c r="E36" s="17">
+        <v>9825007333</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>329</v>
+        <v>236</v>
+      </c>
+      <c r="E37" s="17">
+        <v>9824403400</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="E38" s="17">
-        <v>9825007333</v>
+        <v>98241293358</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" s="17">
-        <v>9824403400</v>
+        <v>249</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="E40" s="17">
-        <v>98241293358</v>
+        <v>9414403681</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>327</v>
+        <v>71</v>
+      </c>
+      <c r="E41" s="17">
+        <v>9827031443</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="E42" s="17">
-        <v>9414403681</v>
+        <v>9811505425</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>75</v>
+        <v>227</v>
       </c>
       <c r="E43" s="17">
-        <v>9827031443</v>
+        <v>9820221166</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E44" s="17">
-        <v>9811505425</v>
+        <v>97</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="E45" s="17">
-        <v>9820221166</v>
+        <v>9829064400</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
-        <v>45</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>326</v>
+        <v>251</v>
+      </c>
+      <c r="E46" s="17">
+        <v>9810061204</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="E47" s="17">
-        <v>9829064400</v>
+        <v>9718930384</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
-        <v>47</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>281</v>
+        <v>49</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
       <c r="E48" s="17">
-        <v>9810061204</v>
+        <v>9926246887</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="E49" s="17">
-        <v>9718930384</v>
+        <v>9414737035</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="E50" s="17">
-        <v>9926246887</v>
+        <v>8888111999</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>205</v>
+        <v>98</v>
       </c>
       <c r="E51" s="17">
-        <v>9414737035</v>
+        <v>8805002505</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
       <c r="E52" s="17">
-        <v>8888111999</v>
+        <v>9822056066</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E53" s="17">
-        <v>8805002505</v>
+        <v>9822094737</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="E54" s="17">
-        <v>9822056066</v>
+        <v>9823023051</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="E55" s="17">
-        <v>9822094737</v>
+        <v>98220273336</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
-        <v>55</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>41</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="E56" s="17">
-        <v>9823023051</v>
+        <v>9822242791</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>277</v>
+        <v>41</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E57" s="17">
-        <v>98220273336</v>
+        <v>254</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
-        <v>57</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>278</v>
+        <v>59</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="17">
-        <v>9822242791</v>
+        <v>116</v>
+      </c>
+      <c r="E58" s="15">
+        <v>9425188995</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>317</v>
+        <v>44</v>
+      </c>
+      <c r="E59" s="17">
+        <v>9828039084</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="E60" s="15">
-        <v>9425188995</v>
+        <v>9822024177</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E61" s="17">
-        <v>9828039084</v>
+        <v>255</v>
+      </c>
+      <c r="E61" s="15">
+        <v>9831038670</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="E62" s="15">
-        <v>9822024177</v>
+        <v>9414104567</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="E63" s="15">
-        <v>9831038670</v>
+        <v>9413308480</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="15">
-        <v>9414104567</v>
+        <v>241</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="E65" s="15">
-        <v>9413308480</v>
+        <v>9414164671</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D66" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>308</v>
+        <v>108</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="E66" s="15">
+        <v>9829266576</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
       <c r="E67" s="15">
-        <v>9414164671</v>
+        <v>9414156680</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>293</v>
+        <v>108</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="E68" s="15">
-        <v>9829266576</v>
+        <v>9784534990</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="E69" s="15">
-        <v>9414156680</v>
+        <v>9879548940</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="E70" s="15">
-        <v>9784534990</v>
+        <v>9823057050</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>245</v>
+        <v>55</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>153</v>
+        <v>256</v>
       </c>
       <c r="E71" s="15">
-        <v>9879548940</v>
+        <v>9818030088</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="E72" s="15">
-        <v>9823057050</v>
+        <v>9829044481</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>155</v>
+        <v>257</v>
       </c>
       <c r="E73" s="15">
-        <v>9818030088</v>
+        <v>7722238440</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="E74" s="15">
-        <v>9829044481</v>
+        <v>242</v>
+      </c>
+      <c r="E74" s="17">
+        <v>9825010151</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="E75" s="15">
-        <v>7722238440</v>
+        <v>9414102255</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E76" s="17">
-        <v>9825010151</v>
+        <v>243</v>
+      </c>
+      <c r="E76" s="15">
+        <v>9829043342</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>158</v>
+        <v>281</v>
       </c>
       <c r="E77" s="15">
-        <v>9414102255</v>
+        <v>9460490980</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D78" s="16" t="s">
-        <v>159</v>
+        <v>258</v>
       </c>
       <c r="E78" s="15">
-        <v>9829043342</v>
+        <v>9829266576</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="13">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D79" s="16" t="s">
-        <v>160</v>
+        <v>259</v>
       </c>
       <c r="E79" s="15">
-        <v>9460490980</v>
+        <v>9826707059</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="13">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="E80" s="15">
-        <v>9829266576</v>
+        <v>9914059108</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="13">
-        <v>80</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>63</v>
+        <v>82</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E81" s="15">
-        <v>9826707059</v>
+        <v>232</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>208</v>
+        <v>270</v>
       </c>
       <c r="E82" s="15">
-        <v>9914059108</v>
+        <v>9893332654</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="13">
-        <v>82</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>279</v>
+        <v>84</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="E83" s="15" t="s">
-        <v>318</v>
+        <v>105</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="13">
-        <v>83</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E84" s="15">
-        <v>9893332654</v>
+        <v>271</v>
+      </c>
+      <c r="E84" s="17">
+        <v>9810341058</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>305</v>
+        <v>260</v>
+      </c>
+      <c r="E85" s="15">
+        <v>9999997513</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13">
-        <v>85</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E86" s="17">
-        <v>9810341058</v>
+        <v>261</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>164</v>
+        <v>262</v>
       </c>
       <c r="E87" s="15">
-        <v>9999997513</v>
+        <v>9303243347</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>309</v>
+        <v>263</v>
+      </c>
+      <c r="E88" s="15">
+        <v>9001361050</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13">
-        <v>88</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E89" s="15">
-        <v>9303243347</v>
+        <v>264</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="E90" s="15">
-        <v>9001361050</v>
+        <v>9702579797</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="13">
-        <v>90</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>68</v>
+        <v>92</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="E91" s="15" t="s">
-        <v>310</v>
+        <v>266</v>
+      </c>
+      <c r="E91" s="15">
+        <v>9001361050</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
-        <v>91</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>227</v>
+        <v>93</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>228</v>
+        <v>272</v>
       </c>
       <c r="E92" s="15">
-        <v>9702579797</v>
+        <v>9414101170</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
-        <v>92</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>275</v>
+        <v>94</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>183</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>165</v>
+        <v>106</v>
       </c>
       <c r="E93" s="15">
-        <v>9001361050</v>
+        <v>9414101395</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E94" s="15">
-        <v>9414101170</v>
+        <v>9929319494</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="13">
-        <v>94</v>
-      </c>
-      <c r="B95" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E95" s="17"/>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="13">
+        <v>97</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D96" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="C95" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D95" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E95" s="15">
-        <v>9414101395</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="13">
-        <v>95</v>
-      </c>
-      <c r="B96" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D96" s="16" t="s">
-        <v>167</v>
-      </c>
       <c r="E96" s="15">
-        <v>9929319494</v>
+        <v>9928085649</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="13">
-        <v>96</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>87</v>
+        <v>98</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>217</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E97" s="17"/>
-    </row>
-    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="E97" s="17">
+        <v>9414103677</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
-        <v>97</v>
-      </c>
-      <c r="B98" s="19" t="s">
-        <v>272</v>
+        <v>99</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E98" s="15">
-        <v>9928085649</v>
+        <v>221</v>
+      </c>
+      <c r="E98" s="17" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="13">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="E99" s="17">
-        <v>9414103677</v>
+        <v>9823151716</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>289</v>
+        <v>267</v>
+      </c>
+      <c r="E100" s="17">
+        <v>9423783830</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="13">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="E101" s="17">
-        <v>9823151716</v>
+        <v>9373831100</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>91</v>
+        <v>187</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E102" s="17">
-        <v>9423783830</v>
+        <v>274</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="13">
-        <v>102</v>
-      </c>
-      <c r="B103" s="16" t="s">
-        <v>92</v>
+        <v>104</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="E103" s="17">
-        <v>9373831100</v>
+        <v>108</v>
+      </c>
+      <c r="D103" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="13">
-        <v>103</v>
-      </c>
-      <c r="B104" s="16" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>319</v>
+        <v>108</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E104" s="15">
+        <v>9413616585</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E105" s="25" t="s">
-        <v>320</v>
+        <v>108</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E105" s="15">
+        <v>9833237000</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="13">
-        <v>105</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>174</v>
+        <v>107</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>175</v>
+        <v>108</v>
+      </c>
+      <c r="D106" s="19" t="s">
+        <v>277</v>
       </c>
       <c r="E106" s="15">
-        <v>9413616585</v>
+        <v>9210034703</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
-        <v>106</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>176</v>
+        <v>108</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>191</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>177</v>
+        <v>108</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="E107" s="15">
-        <v>9833237000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9910303992</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13">
-        <v>107</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E108" s="15">
-        <v>9210034703</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E108" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="F108" s="23"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="13">
-        <v>108</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E109" s="15">
-        <v>9910303992</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E109" s="15"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="13">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>248</v>
+        <v>134</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="E110" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="F110" s="22"/>
+        <v>282</v>
+      </c>
+      <c r="E110" s="15"/>
+      <c r="F110" s="23"/>
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="13">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>249</v>
+        <v>135</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
       <c r="E111" s="15"/>
-      <c r="F111" s="22"/>
+      <c r="F111" s="23"/>
       <c r="G111" s="8"/>
       <c r="H111" s="8"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="13">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>250</v>
+        <v>136</v>
       </c>
       <c r="C112" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>291</v>
+        <v>228</v>
       </c>
       <c r="E112" s="15"/>
-      <c r="F112" s="22"/>
+      <c r="F112" s="23"/>
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="13">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>251</v>
+        <v>137</v>
       </c>
       <c r="C113" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E113" s="15"/>
-      <c r="F113" s="22"/>
+        <v>279</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="F113" s="23"/>
       <c r="G113" s="8"/>
       <c r="H113" s="8"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="13">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>252</v>
+        <v>138</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E114" s="15"/>
-      <c r="F114" s="22"/>
+      <c r="F114" s="23"/>
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="13">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>253</v>
+        <v>139</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="F115" s="22"/>
+        <v>283</v>
+      </c>
+      <c r="E115" s="15">
+        <v>9571913234</v>
+      </c>
+      <c r="F115" s="23"/>
       <c r="G115" s="8"/>
       <c r="H115" s="8"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="13">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>254</v>
+        <v>140</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="E116" s="15"/>
-      <c r="F116" s="22"/>
+        <v>284</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="F116" s="23"/>
       <c r="G116" s="8"/>
       <c r="H116" s="8"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="13">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>255</v>
+        <v>141</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E117" s="15">
-        <v>9571913234</v>
-      </c>
-      <c r="F117" s="22"/>
+        <v>222</v>
+      </c>
+      <c r="E117" s="15"/>
+      <c r="F117" s="23"/>
       <c r="G117" s="8"/>
       <c r="H117" s="8"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="13">
-        <v>117</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>256</v>
+        <v>119</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="E118" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="F118" s="22"/>
+        <v>153</v>
+      </c>
+      <c r="E118" s="15">
+        <v>9414066597</v>
+      </c>
+      <c r="F118" s="23"/>
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="13">
-        <v>118</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C119" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E119" s="15"/>
-      <c r="F119" s="22"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
+        <v>120</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E119" s="15">
+        <v>9425115248</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="13">
-        <v>119</v>
-      </c>
-      <c r="B120" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C120" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="E120" s="15">
-        <v>9414066597</v>
-      </c>
-      <c r="F120" s="22"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C120" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E120" s="15" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="13">
-        <v>120</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>186</v>
+        <v>122</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>194</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>187</v>
+        <v>108</v>
+      </c>
+      <c r="D121" s="19" t="s">
+        <v>286</v>
       </c>
       <c r="E121" s="15">
-        <v>9425115248</v>
+        <v>9302106984</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="13">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>271</v>
+        <v>195</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="E122" s="15" t="s">
-        <v>311</v>
+        <v>118</v>
+      </c>
+      <c r="E122" s="15">
+        <v>9827031575</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="13">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>270</v>
+        <v>196</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D123" s="19" t="s">
-        <v>286</v>
+        <v>108</v>
+      </c>
+      <c r="D123" s="14" t="s">
+        <v>287</v>
       </c>
       <c r="E123" s="15">
-        <v>9302106984</v>
+        <v>9826936900</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="13">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>261</v>
+        <v>197</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>193</v>
+        <v>108</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>289</v>
       </c>
       <c r="E124" s="15">
-        <v>9827031575</v>
+        <v>9425109999</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="13">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>269</v>
+        <v>198</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>194</v>
+        <v>108</v>
+      </c>
+      <c r="D125" s="19" t="s">
+        <v>288</v>
       </c>
       <c r="E125" s="15">
-        <v>9826936900</v>
+        <v>9893229157</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="13">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D126" s="19" t="s">
-        <v>295</v>
+        <v>108</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>290</v>
       </c>
       <c r="E126" s="15">
-        <v>9425109999</v>
+        <v>9822034331</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="13">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D127" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="E127" s="15">
-        <v>9893229157</v>
+        <v>291</v>
+      </c>
+      <c r="E127" s="15" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="13">
-        <v>127</v>
-      </c>
-      <c r="B128" s="14" t="s">
-        <v>213</v>
+        <v>129</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>210</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>214</v>
+        <v>292</v>
       </c>
       <c r="E128" s="15">
-        <v>9822034331</v>
+        <v>9822194024</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="13">
-        <v>128</v>
-      </c>
-      <c r="B129" s="14" t="s">
-        <v>215</v>
+        <v>130</v>
+      </c>
+      <c r="B129" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D129" s="19" t="s">
-        <v>284</v>
+        <v>108</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="E129" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="13">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
       <c r="E130" s="15">
-        <v>9822194024</v>
+        <v>9403007000</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="13">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>264</v>
+        <v>213</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="E131" s="15" t="s">
-        <v>312</v>
+        <v>124</v>
+      </c>
+      <c r="E131" s="15">
+        <v>9822056066</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="13">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>220</v>
+        <v>125</v>
       </c>
       <c r="E132" s="15">
-        <v>9403007000</v>
+        <v>9987111110</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="13">
-        <v>132</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>219</v>
+        <v>134</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>221</v>
+        <v>108</v>
+      </c>
+      <c r="D133" s="19" t="s">
+        <v>297</v>
       </c>
       <c r="E133" s="15">
-        <v>9822056066</v>
+        <v>7977381306</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="13">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D134" s="14" t="s">
-        <v>223</v>
+        <v>108</v>
+      </c>
+      <c r="D134" s="19" t="s">
+        <v>298</v>
       </c>
       <c r="E134" s="15">
-        <v>9987111110</v>
+        <v>9870425586</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="13">
-        <v>134</v>
-      </c>
-      <c r="B135" s="19" t="s">
-        <v>268</v>
+        <v>136</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D135" s="14" t="s">
-        <v>229</v>
+        <v>108</v>
+      </c>
+      <c r="D135" s="19" t="s">
+        <v>295</v>
       </c>
       <c r="E135" s="15">
-        <v>7977381306</v>
+        <v>9076700000</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="13">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>262</v>
+        <v>147</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>230</v>
+        <v>127</v>
       </c>
       <c r="E136" s="15">
-        <v>9870425586</v>
+        <v>9822027336</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="13">
-        <v>136</v>
-      </c>
-      <c r="B137" s="14" t="s">
-        <v>231</v>
+        <v>138</v>
+      </c>
+      <c r="B137" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D137" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="E137" s="15">
-        <v>9076700000</v>
+        <v>128</v>
+      </c>
+      <c r="E137" s="22" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="13">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>232</v>
+        <v>108</v>
+      </c>
+      <c r="D138" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="E138" s="15">
-        <v>9822027336</v>
+        <v>9820293905</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="13">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>234</v>
+        <v>129</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="E139" s="25" t="s">
-        <v>325</v>
+        <v>130</v>
+      </c>
+      <c r="E139" s="15">
+        <v>9323444441</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="13">
-        <v>139</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>236</v>
+        <v>141</v>
+      </c>
+      <c r="B140" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>237</v>
+        <v>130</v>
       </c>
       <c r="E140" s="15">
-        <v>9820293905</v>
+        <v>9820648647</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="13">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D141" s="19" t="s">
-        <v>239</v>
+        <v>108</v>
+      </c>
+      <c r="D141" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="E141" s="15">
-        <v>9323444441</v>
+        <v>9820025899</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="13">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>240</v>
+        <v>144</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D142" s="14" t="s">
-        <v>239</v>
+        <v>108</v>
+      </c>
+      <c r="D142" s="19" t="s">
+        <v>268</v>
       </c>
       <c r="E142" s="15">
-        <v>9820648647</v>
+        <v>7021162267</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="13">
-        <v>142</v>
-      </c>
-      <c r="B143" s="19" t="s">
-        <v>241</v>
+        <v>144</v>
+      </c>
+      <c r="B143" s="21" t="s">
+        <v>145</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E143" s="15">
-        <v>9820025899</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E143" s="15"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="13">
-        <v>143</v>
-      </c>
-      <c r="B144" s="19" t="s">
-        <v>265</v>
+        <v>145</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D144" s="19" t="s">
-        <v>293</v>
-      </c>
-      <c r="E144" s="15">
-        <v>7021162267</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D144" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E144" s="15"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="13">
-        <v>144</v>
-      </c>
-      <c r="B145" s="21" t="s">
-        <v>266</v>
+        <v>146</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E145" s="15"/>
+        <v>108</v>
+      </c>
+      <c r="D145" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E145" s="15">
+        <v>9825010151</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="13">
-        <v>145</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>267</v>
+        <v>147</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E146" s="15"/>
+        <v>108</v>
+      </c>
+      <c r="D146" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="E146" s="15">
+        <v>9825145827</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="13">
-        <v>146</v>
-      </c>
-      <c r="B147" s="14" t="s">
-        <v>244</v>
+        <v>148</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>152</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>243</v>
+        <v>108</v>
+      </c>
+      <c r="D147" s="19" t="s">
+        <v>301</v>
       </c>
       <c r="E147" s="15">
-        <v>9825010151</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="13">
-        <v>147</v>
-      </c>
-      <c r="B148" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D148" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="E148" s="15">
-        <v>9825145827</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="13">
-        <v>148</v>
-      </c>
-      <c r="B149" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="E149" s="15">
         <v>9820229074</v>
       </c>
     </row>

</xml_diff>